<commit_message>
Items into excel and check billno exists script
</commit_message>
<xml_diff>
--- a/Caterogize based on material type.xlsx
+++ b/Caterogize based on material type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IGS\PB Data Utils Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F763810-659B-4931-8D58-D7C3990EB286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BABB4-0CFB-4FC6-BB66-B8085B9461FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{072720D4-D971-4077-8071-E8E78488EDD1}"/>
   </bookViews>
@@ -294,13 +294,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,6 +322,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{31775CE4-6CAA-4424-9428-4B2A07FC8A2D}" name="Table3" displayName="Table3" ref="A1:E22" totalsRowShown="0">
   <autoFilter ref="A1:E22" xr:uid="{31775CE4-6CAA-4424-9428-4B2A07FC8A2D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
+    <sortCondition ref="B1:B22"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{369BAA01-6475-4FF3-B253-58C156D87309}" name="Vendor Po and Invoice"/>
     <tableColumn id="2" xr3:uid="{D93A9097-0682-4AB4-84CA-A35904535BAE}" name="Extra expense"/>
@@ -644,7 +648,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,7 +690,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -713,21 +717,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E3" s="5"/>
       <c r="F3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H3" t="s">
@@ -736,13 +735,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
@@ -750,102 +752,128 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -855,18 +883,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -875,7 +903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>